<commit_message>
Added wrapper for absorption equations
Wrapper functions can be used by WorkingPair-struct
This is for issue #1.
</commit_message>
<xml_diff>
--- a/c_wrapper/data/sorpproplib_ValidationCInterface.xlsx
+++ b/c_wrapper/data/sorpproplib_ValidationCInterface.xlsx
@@ -561,7 +561,7 @@
     <t>refrig</t>
   </si>
   <si>
-    <t>Eric W. Lemmon, Mark O. McLinden and Daniel G. Friend, 'Thermophysical Properties of Fluid Systems' in NIST Chemistry WebBook, NIST Standard Reference Database Number 69, Eds. P.J. Linstrom and W.G. Mallard, National Institute of Standards and Technology, Gaithersburg MD, 20899, https://doi.org/10.18434/T4D303, [Titel anhand dieser DOI in Citavi-Projekt übernehmen]  (retrieved February 14, 2020).</t>
+    <t>Eric W. Lemmon, Mark O. McLinden and Daniel G. Friend, 'Thermophysical Properties of Fluid Systems' in NIST Chemistry WebBook, NIST Standard Reference Database Number 69, Eds. P.J. Linstrom and W.G. Mallard, National Institute of Standards and Technology, Gaithersburg MD, 20899, https://doi.org/10.18434/T4D303, [Titel anhand dieser DOI in Citavi-Projekt übernehmen]  [Titel anhand dieser DOI in Citavi-Projekt übernehmen]  (retrieved February 14, 2020).</t>
   </si>
   <si>
     <t>Refrigerants</t>
@@ -1221,13 +1221,13 @@
     <t>0.2097</t>
   </si>
   <si>
-    <t>6.01814</t>
-  </si>
-  <si>
-    <t>-1.203835</t>
-  </si>
-  <si>
-    <t>-53.226</t>
+    <t>4.72583</t>
+  </si>
+  <si>
+    <t>1660.652</t>
+  </si>
+  <si>
+    <t>-1.461</t>
   </si>
   <si>
     <t>mof</t>

</xml_diff>